<commit_message>
Updated BOM and schematics
</commit_message>
<xml_diff>
--- a/H41R60/Released/BOM/H41R60.xlsx
+++ b/H41R60/Released/BOM/H41R60.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Hexabitz\Hardware\Eagle\design-automation\Modules\H41R60\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hexabitz_Github\Hardware\H41R6x-Hardware\H41R60\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0D91CC-90DD-4057-BD35-874F7A539011}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC21E4F8-E794-4BEA-BF47-8DE4C3347494}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-30" windowWidth="23025" windowHeight="4335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t xml:space="preserve">STMicroelectronics </t>
   </si>
   <si>
-    <t>https://octopart.com/stm32f091cbu6-stmicroelectronics-51988677?r=sp&amp;s=bU6fpgsrTZOxHyt7jkfh3w</t>
-  </si>
-  <si>
     <t>0.0R</t>
   </si>
   <si>
@@ -276,6 +273,9 @@
   </si>
   <si>
     <t>ARM Cortex-M4 STM32F4 Microcontroller IC 32-Bit 100MHz 1.5MB (1.5M x 8) FLASH 100-LQFP (14x14)</t>
+  </si>
+  <si>
+    <t>https://octopart.com/stm32f413vht6-stmicroelectronics-75832293?r=sp&amp;s=_e4TXIFmR5mlyuiVVXP48A</t>
   </si>
 </sst>
 </file>
@@ -712,31 +712,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="60.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="90.5703125" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.265625" customWidth="1"/>
+    <col min="2" max="2" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3984375" customWidth="1"/>
+    <col min="4" max="4" width="60.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="90.59765625" customWidth="1"/>
+    <col min="8" max="8" width="6.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -754,284 +754,287 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="6" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.5">
       <c r="A2" s="4">
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G9" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A12" s="1">
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>50</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G12" r:id="rId1" xr:uid="{6803A2F1-82A0-4CF8-B20A-BB3680AE7530}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>